<commit_message>
Marked FUL_Transmittals_New_Correspondence for execution
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FULPP_WS\Fulcrum_PreProd_Trunk\src\com\proj\suite\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15255" windowHeight="3105"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -485,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Included test - FUL_Transmittals_ActionRequired_New_ChangeNote
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreProdWS\Fulcrum_PreProd_Trunk\src\com\proj\suite\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15255" windowHeight="3105"/>
   </bookViews>
@@ -10,12 +15,11 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>TCID</t>
   </si>
@@ -48,12 +52,18 @@
   </si>
   <si>
     <t>Creates a new Transmittal of  Correspondence</t>
+  </si>
+  <si>
+    <t>FUL_Transmittals_ActionRequired_New_ChangeNote</t>
+  </si>
+  <si>
+    <t>Creates a new Transmittal of  Change Note and validate the count in Action Require</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -479,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -532,12 +542,30 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D3">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
FUL_Transmittals_ActionOverDue_New_ChangeNote marked for execution
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>TCID</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Creates a new Transmittal of  Change Note and validate the count in Action Require</t>
+  </si>
+  <si>
+    <t>FUL_Transmittals_ActionOverDue_New_ChangeNote</t>
+  </si>
+  <si>
+    <t>Creates a new Transmittal of  Change Note and validate the count in Action Overdue</t>
   </si>
 </sst>
 </file>
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -560,12 +566,30 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D4">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>